<commit_message>
jó excel már kajakra
</commit_message>
<xml_diff>
--- a/resources/terkep_adatok_2.xlsx
+++ b/resources/terkep_adatok_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="8690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="8690"/>
   </bookViews>
   <sheets>
     <sheet name="adatok" sheetId="1" r:id="rId1"/>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6519,7 +6519,7 @@
         <v>10</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -6563,7 +6563,7 @@
         <v>10</v>
       </c>
       <c r="E120">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F120">
         <v>2</v>
@@ -6609,7 +6609,7 @@
         <v>10</v>
       </c>
       <c r="E121">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F121">
         <v>3</v>
@@ -6655,7 +6655,7 @@
         <v>10</v>
       </c>
       <c r="E122">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -6701,7 +6701,7 @@
         <v>10</v>
       </c>
       <c r="E123">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F123">
         <v>5</v>
@@ -6747,7 +6747,7 @@
         <v>10</v>
       </c>
       <c r="E124">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F124">
         <v>6</v>
@@ -6793,7 +6793,7 @@
         <v>10</v>
       </c>
       <c r="E125">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F125">
         <v>7</v>
@@ -6839,7 +6839,7 @@
         <v>10</v>
       </c>
       <c r="E126">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F126">
         <v>8</v>
@@ -6885,7 +6885,7 @@
         <v>10</v>
       </c>
       <c r="E127">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F127">
         <v>8</v>
@@ -6931,7 +6931,7 @@
         <v>10</v>
       </c>
       <c r="E128">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F128">
         <v>7</v>
@@ -6977,7 +6977,7 @@
         <v>10</v>
       </c>
       <c r="E129">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -7023,7 +7023,7 @@
         <v>10</v>
       </c>
       <c r="E130">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F130">
         <v>5</v>
@@ -7069,7 +7069,7 @@
         <v>10</v>
       </c>
       <c r="E131">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F131">
         <v>4</v>
@@ -7115,7 +7115,7 @@
         <v>10</v>
       </c>
       <c r="E132">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F132">
         <v>3</v>
@@ -7161,7 +7161,7 @@
         <v>10</v>
       </c>
       <c r="E133">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F133">
         <v>2</v>
@@ -7207,7 +7207,7 @@
         <v>10</v>
       </c>
       <c r="E134">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F134">
         <v>1</v>
@@ -7251,7 +7251,7 @@
         <v>11</v>
       </c>
       <c r="E135">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -7297,7 +7297,7 @@
         <v>11</v>
       </c>
       <c r="E136">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F136">
         <v>2</v>
@@ -7343,7 +7343,7 @@
         <v>11</v>
       </c>
       <c r="E137">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F137">
         <v>3</v>
@@ -7389,7 +7389,7 @@
         <v>11</v>
       </c>
       <c r="E138">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F138">
         <v>4</v>
@@ -7435,7 +7435,7 @@
         <v>11</v>
       </c>
       <c r="E139">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F139">
         <v>5</v>
@@ -7481,7 +7481,7 @@
         <v>11</v>
       </c>
       <c r="E140">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F140">
         <v>6</v>
@@ -7527,7 +7527,7 @@
         <v>11</v>
       </c>
       <c r="E141">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F141">
         <v>7</v>
@@ -7573,7 +7573,7 @@
         <v>11</v>
       </c>
       <c r="E142">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F142">
         <v>7</v>
@@ -7619,7 +7619,7 @@
         <v>11</v>
       </c>
       <c r="E143">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F143">
         <v>7</v>
@@ -7665,7 +7665,7 @@
         <v>11</v>
       </c>
       <c r="E144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F144">
         <v>6</v>
@@ -7711,7 +7711,7 @@
         <v>11</v>
       </c>
       <c r="E145">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F145">
         <v>5</v>
@@ -7757,7 +7757,7 @@
         <v>11</v>
       </c>
       <c r="E146">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F146">
         <v>4</v>
@@ -7803,7 +7803,7 @@
         <v>11</v>
       </c>
       <c r="E147">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F147">
         <v>3</v>
@@ -7849,7 +7849,7 @@
         <v>11</v>
       </c>
       <c r="E148">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F148">
         <v>2</v>
@@ -7895,7 +7895,7 @@
         <v>11</v>
       </c>
       <c r="E149">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F149">
         <v>1</v>
@@ -7941,7 +7941,7 @@
         <v>12</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F150">
         <v>1</v>
@@ -7985,7 +7985,7 @@
         <v>12</v>
       </c>
       <c r="E151">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -8031,7 +8031,7 @@
         <v>12</v>
       </c>
       <c r="E152">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -8077,7 +8077,7 @@
         <v>12</v>
       </c>
       <c r="E153">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F153">
         <v>4</v>
@@ -8123,7 +8123,7 @@
         <v>12</v>
       </c>
       <c r="E154">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F154">
         <v>5</v>
@@ -8169,7 +8169,7 @@
         <v>12</v>
       </c>
       <c r="E155">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F155">
         <v>6</v>
@@ -8215,7 +8215,7 @@
         <v>12</v>
       </c>
       <c r="E156">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F156">
         <v>6</v>
@@ -8261,7 +8261,7 @@
         <v>12</v>
       </c>
       <c r="E157">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F157">
         <v>6</v>
@@ -8307,7 +8307,7 @@
         <v>12</v>
       </c>
       <c r="E158">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F158">
         <v>6</v>
@@ -8353,7 +8353,7 @@
         <v>12</v>
       </c>
       <c r="E159">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F159">
         <v>5</v>
@@ -8399,7 +8399,7 @@
         <v>12</v>
       </c>
       <c r="E160">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F160">
         <v>4</v>
@@ -8445,7 +8445,7 @@
         <v>12</v>
       </c>
       <c r="E161">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F161">
         <v>3</v>
@@ -8491,7 +8491,7 @@
         <v>12</v>
       </c>
       <c r="E162">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F162">
         <v>2</v>
@@ -8537,7 +8537,7 @@
         <v>12</v>
       </c>
       <c r="E163">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F163">
         <v>1</v>
@@ -8581,7 +8581,7 @@
         <v>13</v>
       </c>
       <c r="E164">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F164">
         <v>1</v>
@@ -8625,7 +8625,7 @@
         <v>13</v>
       </c>
       <c r="E165">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F165">
         <v>2</v>
@@ -8671,7 +8671,7 @@
         <v>13</v>
       </c>
       <c r="E166">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F166">
         <v>3</v>
@@ -8717,7 +8717,7 @@
         <v>13</v>
       </c>
       <c r="E167">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F167">
         <v>4</v>
@@ -8763,7 +8763,7 @@
         <v>13</v>
       </c>
       <c r="E168">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F168">
         <v>5</v>
@@ -8809,7 +8809,7 @@
         <v>13</v>
       </c>
       <c r="E169">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F169">
         <v>5</v>
@@ -8855,7 +8855,7 @@
         <v>13</v>
       </c>
       <c r="E170">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F170">
         <v>5</v>
@@ -8901,7 +8901,7 @@
         <v>13</v>
       </c>
       <c r="E171">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -8947,7 +8947,7 @@
         <v>13</v>
       </c>
       <c r="E172">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F172">
         <v>5</v>
@@ -8993,7 +8993,7 @@
         <v>13</v>
       </c>
       <c r="E173">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F173">
         <v>4</v>
@@ -9039,7 +9039,7 @@
         <v>13</v>
       </c>
       <c r="E174">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F174">
         <v>3</v>
@@ -9085,7 +9085,7 @@
         <v>13</v>
       </c>
       <c r="E175">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F175">
         <v>2</v>
@@ -9131,7 +9131,7 @@
         <v>13</v>
       </c>
       <c r="E176">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F176">
         <v>1</v>
@@ -9175,7 +9175,7 @@
         <v>14</v>
       </c>
       <c r="E177">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F177">
         <v>1</v>
@@ -9219,7 +9219,7 @@
         <v>14</v>
       </c>
       <c r="E178">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F178">
         <v>2</v>
@@ -9265,7 +9265,7 @@
         <v>14</v>
       </c>
       <c r="E179">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F179">
         <v>3</v>
@@ -9311,7 +9311,7 @@
         <v>14</v>
       </c>
       <c r="E180">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F180">
         <v>4</v>
@@ -9357,7 +9357,7 @@
         <v>14</v>
       </c>
       <c r="E181">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F181">
         <v>4</v>
@@ -9403,7 +9403,7 @@
         <v>14</v>
       </c>
       <c r="E182">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F182">
         <v>4</v>
@@ -9449,7 +9449,7 @@
         <v>14</v>
       </c>
       <c r="E183">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F183">
         <v>4</v>
@@ -9495,7 +9495,7 @@
         <v>14</v>
       </c>
       <c r="E184">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F184">
         <v>4</v>
@@ -9541,7 +9541,7 @@
         <v>14</v>
       </c>
       <c r="E185">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F185">
         <v>4</v>
@@ -9587,7 +9587,7 @@
         <v>14</v>
       </c>
       <c r="E186">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F186">
         <v>3</v>
@@ -9633,7 +9633,7 @@
         <v>14</v>
       </c>
       <c r="E187">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F187">
         <v>2</v>
@@ -9679,7 +9679,7 @@
         <v>14</v>
       </c>
       <c r="E188">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F188">
         <v>1</v>
@@ -9723,7 +9723,7 @@
         <v>15</v>
       </c>
       <c r="E189">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F189">
         <v>1</v>
@@ -9769,7 +9769,7 @@
         <v>15</v>
       </c>
       <c r="E190">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F190">
         <v>2</v>
@@ -9815,7 +9815,7 @@
         <v>15</v>
       </c>
       <c r="E191">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F191">
         <v>3</v>
@@ -9861,7 +9861,7 @@
         <v>15</v>
       </c>
       <c r="E192">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F192">
         <v>3</v>
@@ -9907,7 +9907,7 @@
         <v>15</v>
       </c>
       <c r="E193">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F193">
         <v>3</v>
@@ -9953,7 +9953,7 @@
         <v>15</v>
       </c>
       <c r="E194">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F194">
         <v>3</v>
@@ -9999,7 +9999,7 @@
         <v>15</v>
       </c>
       <c r="E195">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F195">
         <v>3</v>
@@ -10045,7 +10045,7 @@
         <v>15</v>
       </c>
       <c r="E196">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F196">
         <v>3</v>
@@ -10091,7 +10091,7 @@
         <v>15</v>
       </c>
       <c r="E197">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F197">
         <v>3</v>
@@ -10137,7 +10137,7 @@
         <v>15</v>
       </c>
       <c r="E198">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F198">
         <v>2</v>
@@ -10183,7 +10183,7 @@
         <v>15</v>
       </c>
       <c r="E199">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F199">
         <v>1</v>
@@ -10229,7 +10229,7 @@
         <v>16</v>
       </c>
       <c r="E200">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F200">
         <v>1</v>
@@ -10273,7 +10273,7 @@
         <v>16</v>
       </c>
       <c r="E201">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F201">
         <v>2</v>
@@ -10319,7 +10319,7 @@
         <v>16</v>
       </c>
       <c r="E202">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F202">
         <v>2</v>
@@ -10365,7 +10365,7 @@
         <v>16</v>
       </c>
       <c r="E203">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F203">
         <v>2</v>
@@ -10411,7 +10411,7 @@
         <v>16</v>
       </c>
       <c r="E204">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F204">
         <v>2</v>
@@ -10457,7 +10457,7 @@
         <v>16</v>
       </c>
       <c r="E205">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F205">
         <v>2</v>
@@ -10503,7 +10503,7 @@
         <v>16</v>
       </c>
       <c r="E206">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F206">
         <v>2</v>
@@ -10549,7 +10549,7 @@
         <v>16</v>
       </c>
       <c r="E207">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F207">
         <v>2</v>
@@ -10595,7 +10595,7 @@
         <v>16</v>
       </c>
       <c r="E208">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F208">
         <v>2</v>
@@ -10641,7 +10641,7 @@
         <v>16</v>
       </c>
       <c r="E209">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F209">
         <v>1</v>
@@ -10685,7 +10685,7 @@
         <v>17</v>
       </c>
       <c r="E210">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F210">
         <v>1</v>
@@ -10729,7 +10729,7 @@
         <v>17</v>
       </c>
       <c r="E211">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F211">
         <v>1</v>
@@ -10773,7 +10773,7 @@
         <v>17</v>
       </c>
       <c r="E212">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F212">
         <v>1</v>
@@ -10819,7 +10819,7 @@
         <v>17</v>
       </c>
       <c r="E213">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F213">
         <v>1</v>
@@ -10863,7 +10863,7 @@
         <v>17</v>
       </c>
       <c r="E214">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F214">
         <v>1</v>
@@ -10907,7 +10907,7 @@
         <v>17</v>
       </c>
       <c r="E215">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F215">
         <v>1</v>
@@ -10951,7 +10951,7 @@
         <v>17</v>
       </c>
       <c r="E216">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F216">
         <v>1</v>
@@ -10997,7 +10997,7 @@
         <v>17</v>
       </c>
       <c r="E217">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F217">
         <v>1</v>
@@ -11041,7 +11041,7 @@
         <v>17</v>
       </c>
       <c r="E218">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F218">
         <v>1</v>
@@ -15494,7 +15494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Új víz adatok az excelben
</commit_message>
<xml_diff>
--- a/resources/terkep_adatok_2.xlsx
+++ b/resources/terkep_adatok_2.xlsx
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:Q218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="O4">
         <f>(F4-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L4,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -1447,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="O8">
         <f>(F8-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L8,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
@@ -2037,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="O21">
         <f>(F21-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L21,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q21" s="1"/>
     </row>
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="O31">
         <f>(F31-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L31,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q31" s="1"/>
     </row>
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H71" s="1">
         <v>0</v>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="O71">
         <f>(F71-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L71,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q71" s="1"/>
     </row>
@@ -4969,7 +4969,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H85" s="1">
         <v>0</v>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="O85">
         <f>(F85-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L85,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q85" s="1"/>
     </row>
@@ -7257,7 +7257,7 @@
         <v>1</v>
       </c>
       <c r="G135" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H135" s="1">
         <v>0</v>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="O135">
         <f>(F135-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L135,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q135" s="1"/>
     </row>
@@ -7901,7 +7901,7 @@
         <v>1</v>
       </c>
       <c r="G149" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H149" s="1">
         <v>0</v>
@@ -7923,7 +7923,7 @@
       </c>
       <c r="O149">
         <f>(F149-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L149,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q149" s="1"/>
     </row>
@@ -9729,7 +9729,7 @@
         <v>1</v>
       </c>
       <c r="G189" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H189" s="1">
         <v>0</v>
@@ -9751,7 +9751,7 @@
       </c>
       <c r="O189">
         <f>(F189-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L189,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q189" s="1"/>
     </row>
@@ -10189,7 +10189,7 @@
         <v>1</v>
       </c>
       <c r="G199" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H199" s="1">
         <v>0</v>
@@ -10211,7 +10211,7 @@
       </c>
       <c r="O199">
         <f>(F199-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L199,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q199" s="1"/>
     </row>
@@ -10779,7 +10779,7 @@
         <v>1</v>
       </c>
       <c r="G212" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H212" s="1">
         <v>0</v>
@@ -10801,7 +10801,7 @@
       </c>
       <c r="O212">
         <f>(F212-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L212,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q212" s="1"/>
     </row>
@@ -10957,7 +10957,7 @@
         <v>1</v>
       </c>
       <c r="G216" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H216" s="1">
         <v>0</v>
@@ -10979,7 +10979,7 @@
       </c>
       <c r="O216">
         <f>(F216-1)*segédtbl!F$2+segédtbl!F$3+VLOOKUP(adatok!L216,segédtbl!B$2:C$5,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q216" s="1"/>
     </row>
@@ -11081,7 +11081,7 @@
   <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11105,7 +11105,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>238</v>

</xml_diff>